<commit_message>
start rough work for task 1 and update semester plan.
</commit_message>
<xml_diff>
--- a/rough_work_and_planning/sem_4_plan.xlsx
+++ b/rough_work_and_planning/sem_4_plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="124">
   <si>
     <t xml:space="preserve">? Reading Week - TBC</t>
   </si>
@@ -127,6 +127,9 @@
     <t xml:space="preserve">10 mins</t>
   </si>
   <si>
+    <t xml:space="preserve">Week 3 – update weekly plan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Applied Statistics</t>
   </si>
   <si>
@@ -190,10 +193,10 @@
     <t xml:space="preserve">Lectures</t>
   </si>
   <si>
-    <t xml:space="preserve">1.02.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction</t>
+    <t xml:space="preserve">2.02.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch introduction lectures</t>
   </si>
   <si>
     <t xml:space="preserve">1.5hr</t>
@@ -202,142 +205,160 @@
     <t xml:space="preserve">1.02.2</t>
   </si>
   <si>
+    <t xml:space="preserve">Watch assessments lectures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topic 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.03.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permutations and Combinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.03.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numpy's Normal Distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.03.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-Test Calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.03.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.04.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.04.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 ECTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transcribe notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generalisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch lectures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly Tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.010.10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assessments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TBC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5 hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5hrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.03.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permutations and Combinations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.03.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numpy's Normal Distribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.03.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T-Test Calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.03.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANOVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.04.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Download dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.04.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Machine Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 ECTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linear Regression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5 hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transcribe notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topic 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.010.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.02.1</t>
   </si>
   <si>
     <t xml:space="preserve">MCQ 1</t>
@@ -697,7 +718,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -766,56 +787,80 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1088,14 +1133,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CT238"/>
+  <dimension ref="A1:CT251"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="O19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="O55" activeCellId="0" sqref="O55"/>
+      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="V5" activeCellId="0" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1905,13 +1950,13 @@
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="18" t="n">
+      <c r="F7" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1923,13 +1968,13 @@
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="18" t="n">
+      <c r="F8" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1941,1302 +1986,1442 @@
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="18" t="n">
+      <c r="F9" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="O9" s="18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="n">
+      <c r="A10" s="1" t="n">
+        <f aca="false">A9+0.01</f>
+        <v>1.04</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="W10" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="n">
         <f aca="false">A6+1</f>
         <v>2</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="20" t="s">
+      <c r="B12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="n">
-        <f aca="false">A11+0.01</f>
+      <c r="C12" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23" t="n">
+        <f aca="false">A12+0.01</f>
         <v>2.01</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="s">
+      <c r="B14" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="24" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="18" t="n">
+      <c r="E15" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
+      <c r="H15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="24" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="18" t="n">
+      <c r="B16" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="24" t="s">
+      <c r="H16" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="18" t="n">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="L16" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="s">
+      <c r="L17" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="24" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="18" t="n">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="L17" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="s">
+      <c r="L18" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="24" t="s">
+      <c r="E19" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="18" t="n">
+      <c r="F19" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="L19" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="24" t="s">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24" t="s">
+      <c r="B20" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="18" t="n">
+      <c r="F20" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="O19" s="19" t="s">
+      <c r="O20" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="24" t="s">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24" t="s">
+      <c r="B21" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="25"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="n">
-        <f aca="false">A13+0.01</f>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="26"/>
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="23" t="n">
+        <f aca="false">A14+0.01</f>
         <v>2.02</v>
       </c>
-      <c r="B22" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24" t="s">
+      <c r="B23" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="B24" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="18" t="n">
+      <c r="E24" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="H23" s="19"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24" t="s">
+      <c r="H24" s="18"/>
+    </row>
+    <row r="25" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="33"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="18" t="n">
+      <c r="F26" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="O24" s="19" t="s">
+      <c r="O26" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="28"/>
+      <c r="B27" s="25"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="31"/>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="18"/>
-      <c r="V25" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="24" t="s">
+      <c r="E28" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="W28" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="18"/>
-      <c r="AC26" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="24" t="s">
+    </row>
+    <row r="29" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="31"/>
+      <c r="B29" s="28"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="31"/>
+      <c r="V29" s="34"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="AJ27" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="24" t="s">
+      <c r="D30" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="AC30" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="31"/>
+      <c r="B31" s="28"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="31"/>
+      <c r="AC31" s="34"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="18"/>
-      <c r="AX28" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="24" t="s">
+      <c r="D32" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="AJ32" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="31"/>
+      <c r="B33" s="28"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="31"/>
+      <c r="AJ33" s="34"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="18"/>
-      <c r="BE29" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="24" t="s">
+      <c r="D34" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="AX34" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="31"/>
+      <c r="B35" s="28"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="31"/>
+      <c r="AX35" s="34"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F30" s="18"/>
-      <c r="BL30" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="24" t="s">
+      <c r="D36" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="BE36" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="31"/>
+      <c r="B37" s="28"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="31"/>
+      <c r="BE37" s="34"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="18"/>
-      <c r="BR31" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="BS31" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="24" t="s">
+      <c r="D38" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="BL38" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="31"/>
+      <c r="B39" s="28"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="31"/>
+      <c r="BL39" s="34"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" s="18"/>
-      <c r="BZ32" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="21"/>
-      <c r="F33" s="18"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="21"/>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="21"/>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="22" t="n">
-        <f aca="false">A22+0.01</f>
+      <c r="D40" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="17"/>
+      <c r="BR40" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="BS40" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" s="30" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="31"/>
+      <c r="B41" s="28"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="31"/>
+      <c r="BR41" s="34"/>
+      <c r="BS41" s="34"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="BZ42" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="22"/>
+      <c r="F43" s="17"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="22"/>
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="22"/>
+      <c r="F45" s="17"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="23" t="n">
+        <f aca="false">A23+0.01</f>
         <v>2.03</v>
       </c>
-      <c r="B36" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25" t="s">
+      <c r="B46" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="F46" s="17"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="25" t="s">
+      <c r="B47" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="F47" s="17"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F48" s="17"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="25" t="s">
+      <c r="B49" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="F49" s="17"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F50" s="17"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25" t="s">
+      <c r="B51" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="29" t="s">
+      <c r="F51" s="17"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F52" s="17"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F44" s="18"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F45" s="18"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="22" t="n">
-        <f aca="false">A36+0.01</f>
+      <c r="B53" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" s="17"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F54" s="17"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F55" s="17"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="23" t="n">
+        <f aca="false">A46+0.01</f>
         <v>2.04</v>
       </c>
-      <c r="B46" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="24" t="s">
+      <c r="B56" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="F56" s="17"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="18" t="n">
+      <c r="B57" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F57" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="K47" s="19"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" s="24" t="s">
+      <c r="K57" s="18"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24" t="s">
+      <c r="B58" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="F48" s="18"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F49" s="18"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F50" s="18"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="n">
-        <f aca="false">A11+1</f>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F58" s="17"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F59" s="17"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F60" s="17"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="14" t="n">
+        <f aca="false">A12+1</f>
         <v>3</v>
       </c>
-      <c r="B51" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C51" s="20" t="s">
+      <c r="B61" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="18"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="22" t="n">
+      <c r="C61" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="17"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="23" t="n">
         <f aca="false">2+0.01</f>
         <v>2.01</v>
       </c>
-      <c r="B53" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F53" s="18"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="B54" s="29" t="s">
+      <c r="B63" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F63" s="17"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E54" s="24" t="s">
+      <c r="B64" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="F54" s="18" t="n">
+      <c r="E64" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F64" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="L54" s="19" t="s">
+      <c r="L64" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="E65" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="F65" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="P65" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" s="16"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="17"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D67" s="16"/>
+      <c r="E67" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F67" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="T67" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F68" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="T68" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D69" s="16"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="17"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B70" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E70" s="25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="30" t="s">
+      <c r="F70" s="17"/>
+      <c r="Z70" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" s="30" t="s">
+    </row>
+    <row r="71" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F55" s="18"/>
-      <c r="P55" s="27" t="s">
+      <c r="E71" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F71" s="17"/>
+      <c r="AG71" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="D56" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F56" s="18"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B57" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E57" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F57" s="18"/>
-      <c r="S57" s="27" t="s">
+      <c r="E72" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="Z57" s="27" t="s">
+      <c r="F72" s="17"/>
+      <c r="AN72" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E73" s="25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F58" s="18"/>
-      <c r="AG58" s="27" t="s">
+      <c r="F73" s="17"/>
+      <c r="BB73" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B74" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E74" s="25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B59" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="D59" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F59" s="18"/>
-      <c r="AN59" s="27" t="s">
+      <c r="F74" s="17"/>
+      <c r="BI74" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B75" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E75" s="25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B60" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D60" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F60" s="18"/>
-      <c r="BB60" s="27" t="s">
+      <c r="F75" s="17"/>
+      <c r="BP75" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B76" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E76" s="25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B61" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D61" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F61" s="18"/>
-      <c r="BI61" s="27" t="s">
+      <c r="F76" s="17"/>
+      <c r="BW76" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E77" s="25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="B62" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D62" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F62" s="18"/>
-      <c r="BP62" s="27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B63" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D63" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F63" s="18"/>
-      <c r="BW63" s="27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D64" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F64" s="18"/>
-      <c r="CD64" s="27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F65" s="18"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F66" s="18"/>
-    </row>
-    <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="22" t="n">
-        <f aca="false">A53+0.01</f>
+      <c r="F77" s="17"/>
+      <c r="CD77" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F78" s="17"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F79" s="17"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="23" t="n">
+        <f aca="false">A63+0.01</f>
         <v>2.02</v>
       </c>
-      <c r="B67" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F67" s="18"/>
-    </row>
-    <row r="68" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="B69" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B70" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F71" s="18"/>
-    </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F72" s="18"/>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="14" t="n">
-        <f aca="false">A51+1</f>
+      <c r="B80" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F80" s="17"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B81" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B82" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="25"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B83" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="25"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F84" s="17"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F85" s="17"/>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="14" t="n">
+        <f aca="false">A61+1</f>
         <v>4</v>
       </c>
-      <c r="B73" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="F73" s="18"/>
-    </row>
-    <row r="74" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="25" t="n">
-        <f aca="false">A73+0.01</f>
+      <c r="B86" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="F86" s="17"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="26" t="n">
+        <f aca="false">A86+0.01</f>
         <v>4.01</v>
       </c>
-      <c r="B74" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74" s="31"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="26" t="s">
+      <c r="B87" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87" s="37"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F74" s="18" t="n">
+      <c r="F87" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="L74" s="19" t="s">
+      <c r="L87" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="25" t="n">
-        <f aca="false">A74+0.01</f>
+    <row r="88" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="26" t="n">
+        <f aca="false">A87+0.01</f>
         <v>4.02</v>
       </c>
-      <c r="B75" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="E75" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="F75" s="18" t="n">
+      <c r="B88" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E88" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F88" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="L75" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="25" t="n">
-        <f aca="false">A75+0.01</f>
+      <c r="L88" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="26" t="n">
+        <f aca="false">A88+0.01</f>
         <v>4.03</v>
       </c>
-      <c r="B76" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="F76" s="18"/>
-    </row>
-    <row r="77" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="25" t="n">
-        <f aca="false">A76+0.01</f>
+      <c r="B89" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="F89" s="17"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="26" t="n">
+        <f aca="false">A89+0.01</f>
         <v>4.04</v>
       </c>
-      <c r="B77" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="F77" s="18"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F78" s="18"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F79" s="18"/>
-    </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F80" s="18"/>
-    </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F81" s="18"/>
-    </row>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F82" s="18"/>
-    </row>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F83" s="18"/>
-    </row>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F84" s="18"/>
-    </row>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F85" s="18"/>
-    </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F86" s="18"/>
-    </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F87" s="18"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F88" s="18"/>
-    </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F89" s="18"/>
-    </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F90" s="18"/>
+      <c r="B90" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="F90" s="17"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F91" s="18"/>
+      <c r="F91" s="17"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F92" s="18"/>
+      <c r="F92" s="17"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F93" s="18"/>
+      <c r="F93" s="17"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F94" s="18"/>
+      <c r="F94" s="17"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F95" s="18"/>
+      <c r="F95" s="17"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F96" s="18"/>
+      <c r="F96" s="17"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F97" s="18"/>
+      <c r="F97" s="17"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F98" s="18"/>
+      <c r="F98" s="17"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F99" s="18"/>
+      <c r="F99" s="17"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F100" s="18"/>
+      <c r="F100" s="17"/>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F101" s="18"/>
+      <c r="F101" s="17"/>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F102" s="18"/>
+      <c r="F102" s="17"/>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F103" s="18"/>
+      <c r="F103" s="17"/>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F104" s="18"/>
+      <c r="F104" s="17"/>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F105" s="18"/>
+      <c r="F105" s="17"/>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F106" s="18"/>
+      <c r="F106" s="17"/>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F107" s="18"/>
+      <c r="F107" s="17"/>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F108" s="18"/>
+      <c r="F108" s="17"/>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F109" s="18"/>
+      <c r="F109" s="17"/>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F110" s="18"/>
+      <c r="F110" s="17"/>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F111" s="18"/>
+      <c r="F111" s="17"/>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F112" s="18"/>
+      <c r="F112" s="17"/>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F113" s="18"/>
+      <c r="F113" s="17"/>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F114" s="18"/>
+      <c r="F114" s="17"/>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F115" s="18"/>
+      <c r="F115" s="17"/>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F116" s="18"/>
+      <c r="F116" s="17"/>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F117" s="18"/>
+      <c r="F117" s="17"/>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F118" s="18"/>
+      <c r="F118" s="17"/>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F119" s="18"/>
+      <c r="F119" s="17"/>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F120" s="18"/>
+      <c r="F120" s="17"/>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F121" s="18"/>
+      <c r="F121" s="17"/>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F122" s="18"/>
+      <c r="F122" s="17"/>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F123" s="18"/>
+      <c r="F123" s="17"/>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F124" s="18"/>
+      <c r="F124" s="17"/>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F125" s="18"/>
+      <c r="F125" s="17"/>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F126" s="18"/>
+      <c r="F126" s="17"/>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F127" s="18"/>
+      <c r="F127" s="17"/>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F128" s="18"/>
+      <c r="F128" s="17"/>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F129" s="18"/>
+      <c r="F129" s="17"/>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F130" s="18"/>
+      <c r="F130" s="17"/>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F131" s="18"/>
+      <c r="F131" s="17"/>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F132" s="18"/>
+      <c r="F132" s="17"/>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F133" s="18"/>
+      <c r="F133" s="17"/>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F134" s="18"/>
+      <c r="F134" s="17"/>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F135" s="18"/>
+      <c r="F135" s="17"/>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F136" s="18"/>
+      <c r="F136" s="17"/>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F137" s="18"/>
+      <c r="F137" s="17"/>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F138" s="18"/>
+      <c r="F138" s="17"/>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F139" s="18"/>
+      <c r="F139" s="17"/>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F140" s="18"/>
+      <c r="F140" s="17"/>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F141" s="18"/>
+      <c r="F141" s="17"/>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F142" s="18"/>
+      <c r="F142" s="17"/>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F143" s="18"/>
+      <c r="F143" s="17"/>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F144" s="18"/>
+      <c r="F144" s="17"/>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F145" s="18"/>
+      <c r="F145" s="17"/>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F146" s="18"/>
+      <c r="F146" s="17"/>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F147" s="18"/>
+      <c r="F147" s="17"/>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F148" s="18"/>
+      <c r="F148" s="17"/>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F149" s="18"/>
+      <c r="F149" s="17"/>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F150" s="18"/>
+      <c r="F150" s="17"/>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F151" s="18"/>
+      <c r="F151" s="17"/>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F152" s="18"/>
+      <c r="F152" s="17"/>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F153" s="18"/>
+      <c r="F153" s="17"/>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F154" s="18"/>
+      <c r="F154" s="17"/>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F155" s="18"/>
+      <c r="F155" s="17"/>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F156" s="18"/>
+      <c r="F156" s="17"/>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F157" s="18"/>
+      <c r="F157" s="17"/>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F158" s="18"/>
+      <c r="F158" s="17"/>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F159" s="18"/>
+      <c r="F159" s="17"/>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F160" s="18"/>
+      <c r="F160" s="17"/>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F161" s="18"/>
+      <c r="F161" s="17"/>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F162" s="18"/>
+      <c r="F162" s="17"/>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F163" s="18"/>
+      <c r="F163" s="17"/>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F164" s="18"/>
+      <c r="F164" s="17"/>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F165" s="18"/>
+      <c r="F165" s="17"/>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F166" s="18"/>
+      <c r="F166" s="17"/>
     </row>
     <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F167" s="18"/>
+      <c r="F167" s="17"/>
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F168" s="18"/>
+      <c r="F168" s="17"/>
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F169" s="18"/>
+      <c r="F169" s="17"/>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F170" s="18"/>
+      <c r="F170" s="17"/>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F171" s="18"/>
+      <c r="F171" s="17"/>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F172" s="18"/>
+      <c r="F172" s="17"/>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F173" s="18"/>
+      <c r="F173" s="17"/>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F174" s="18"/>
+      <c r="F174" s="17"/>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F175" s="18"/>
+      <c r="F175" s="17"/>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F176" s="18"/>
+      <c r="F176" s="17"/>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F177" s="18"/>
+      <c r="F177" s="17"/>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F178" s="18"/>
+      <c r="F178" s="17"/>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F179" s="18"/>
+      <c r="F179" s="17"/>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F180" s="18"/>
+      <c r="F180" s="17"/>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F181" s="18"/>
+      <c r="F181" s="17"/>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F182" s="18"/>
+      <c r="F182" s="17"/>
     </row>
     <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F183" s="18"/>
+      <c r="F183" s="17"/>
     </row>
     <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F184" s="18"/>
+      <c r="F184" s="17"/>
     </row>
     <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F185" s="18"/>
+      <c r="F185" s="17"/>
     </row>
     <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F186" s="18"/>
+      <c r="F186" s="17"/>
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F187" s="18"/>
+      <c r="F187" s="17"/>
     </row>
     <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F188" s="18"/>
+      <c r="F188" s="17"/>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F189" s="18"/>
+      <c r="F189" s="17"/>
     </row>
     <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F190" s="18"/>
+      <c r="F190" s="17"/>
     </row>
     <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F191" s="18"/>
+      <c r="F191" s="17"/>
     </row>
     <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F192" s="18"/>
+      <c r="F192" s="17"/>
     </row>
     <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F193" s="18"/>
+      <c r="F193" s="17"/>
     </row>
     <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F194" s="18"/>
+      <c r="F194" s="17"/>
     </row>
     <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F195" s="18"/>
+      <c r="F195" s="17"/>
     </row>
     <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F196" s="18"/>
+      <c r="F196" s="17"/>
     </row>
     <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F197" s="18"/>
+      <c r="F197" s="17"/>
     </row>
     <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F198" s="18"/>
+      <c r="F198" s="17"/>
     </row>
     <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F199" s="18"/>
+      <c r="F199" s="17"/>
     </row>
     <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F200" s="18"/>
+      <c r="F200" s="17"/>
     </row>
     <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F201" s="18"/>
+      <c r="F201" s="17"/>
     </row>
     <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F202" s="18"/>
+      <c r="F202" s="17"/>
     </row>
     <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F203" s="18"/>
+      <c r="F203" s="17"/>
     </row>
     <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F204" s="18"/>
+      <c r="F204" s="17"/>
     </row>
     <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F205" s="18"/>
+      <c r="F205" s="17"/>
     </row>
     <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F206" s="18"/>
+      <c r="F206" s="17"/>
     </row>
     <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F207" s="18"/>
+      <c r="F207" s="17"/>
     </row>
     <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F208" s="18"/>
+      <c r="F208" s="17"/>
     </row>
     <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F209" s="18"/>
+      <c r="F209" s="17"/>
     </row>
     <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F210" s="18"/>
+      <c r="F210" s="17"/>
     </row>
     <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F211" s="18"/>
+      <c r="F211" s="17"/>
     </row>
     <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F212" s="18"/>
+      <c r="F212" s="17"/>
     </row>
     <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F213" s="18"/>
+      <c r="F213" s="17"/>
     </row>
     <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F214" s="18"/>
+      <c r="F214" s="17"/>
     </row>
     <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F215" s="18"/>
+      <c r="F215" s="17"/>
     </row>
     <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F216" s="18"/>
+      <c r="F216" s="17"/>
     </row>
     <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F217" s="18"/>
+      <c r="F217" s="17"/>
     </row>
     <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F218" s="18"/>
+      <c r="F218" s="17"/>
     </row>
     <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F219" s="18"/>
+      <c r="F219" s="17"/>
     </row>
     <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F220" s="18"/>
+      <c r="F220" s="17"/>
     </row>
     <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F221" s="18"/>
+      <c r="F221" s="17"/>
     </row>
     <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F222" s="18"/>
+      <c r="F222" s="17"/>
     </row>
     <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F223" s="18"/>
+      <c r="F223" s="17"/>
     </row>
     <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F224" s="18"/>
+      <c r="F224" s="17"/>
     </row>
     <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F225" s="18"/>
+      <c r="F225" s="17"/>
     </row>
     <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F226" s="18"/>
+      <c r="F226" s="17"/>
     </row>
     <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F227" s="18"/>
+      <c r="F227" s="17"/>
     </row>
     <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F228" s="18"/>
+      <c r="F228" s="17"/>
     </row>
     <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F229" s="18"/>
+      <c r="F229" s="17"/>
     </row>
     <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F230" s="18"/>
+      <c r="F230" s="17"/>
     </row>
     <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F231" s="18"/>
+      <c r="F231" s="17"/>
     </row>
     <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F232" s="18"/>
+      <c r="F232" s="17"/>
     </row>
     <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F233" s="18"/>
+      <c r="F233" s="17"/>
     </row>
     <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F234" s="18"/>
+      <c r="F234" s="17"/>
     </row>
     <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F235" s="18"/>
+      <c r="F235" s="17"/>
     </row>
     <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F236" s="18"/>
+      <c r="F236" s="17"/>
     </row>
     <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F237" s="18"/>
+      <c r="F237" s="17"/>
     </row>
     <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F238" s="18"/>
+      <c r="F238" s="17"/>
+    </row>
+    <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F239" s="17"/>
+    </row>
+    <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F240" s="17"/>
+    </row>
+    <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F241" s="17"/>
+    </row>
+    <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F242" s="17"/>
+    </row>
+    <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F243" s="17"/>
+    </row>
+    <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F244" s="17"/>
+    </row>
+    <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F245" s="17"/>
+    </row>
+    <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F246" s="17"/>
+    </row>
+    <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F247" s="17"/>
+    </row>
+    <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F248" s="17"/>
+    </row>
+    <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F249" s="17"/>
+    </row>
+    <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F250" s="17"/>
+    </row>
+    <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F251" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3255,7 +3440,7 @@
     <mergeCell ref="CG2:CM2"/>
     <mergeCell ref="CN2:CT2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F7:F200">
+  <conditionalFormatting sqref="F7:F213">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="1" minLength="10" maxLength="90">
         <cfvo type="num" val="0"/>
@@ -3264,7 +3449,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B4D841FA-6664-4B79-96AC-DEC430DF1DC5}</x14:id>
+          <x14:id>{32B0FE30-132C-4A43-B53F-2282DBC9F245}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3280,7 +3465,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B4D841FA-6664-4B79-96AC-DEC430DF1DC5}">
+          <x14:cfRule type="dataBar" id="{32B0FE30-132C-4A43-B53F-2282DBC9F245}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3292,7 +3477,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F7:F200</xm:sqref>
+          <xm:sqref>F7:F213</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>